<commit_message>
Replies to SKL inquiries and GenTable updates
</commit_message>
<xml_diff>
--- a/DbLayouts/L1-顧客管理作業/BankRelationSuspected.xlsx
+++ b/DbLayouts/L1-顧客管理作業/BankRelationSuspected.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L1-顧客管理作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L1-顧客管理作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -138,55 +138,55 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>自然人姓名</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustId</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司名稱</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>職務名稱</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepCusNameEq</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepCusName =</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BankRelationSuspected</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepCusName,CustId</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否為疑似準利害關係人檔</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>該自然人擔任董事長之公司統一編號</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>RepCusName</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>自然人姓名</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>該自然人擔任董事長之公司統一編號</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CustId</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RepCusName,CustId</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CustName</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>公司名稱</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>SubCom</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>職務名稱</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RepCusNameEq</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RepCusName =</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否為疑似準利害關係人檔</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>BankRelationSuspected</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -786,7 +786,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -806,10 +806,10 @@
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="10"/>
@@ -913,10 +913,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>32</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>30</v>
@@ -933,10 +933,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>29</v>
@@ -953,10 +953,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>30</v>
@@ -973,10 +973,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>30</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="2" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>